<commit_message>
Tutorial blocks were added
</commit_message>
<xml_diff>
--- a/psychopy_experiment/comp_materials/passage_qa/questionbank.xlsx
+++ b/psychopy_experiment/comp_materials/passage_qa/questionbank.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erang\Desktop\Reading_task\psychopy_experiment\comp_materials\passage_qa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C55EC5E5-6F94-46DA-BD1E-759D4293A098}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E774C1A-7034-4B8B-8EE8-C48072A1B3F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="54">
   <si>
     <t>R1</t>
   </si>
@@ -182,16 +182,82 @@
   </si>
   <si>
     <t>2. By the late sixth century BC, what did the vision of the ideal citizen of the city-state lead to?</t>
+  </si>
+  <si>
+    <t>practice1</t>
+  </si>
+  <si>
+    <t>practice2</t>
+  </si>
+  <si>
+    <t>1.Where was the city of Oceana located?</t>
+  </si>
+  <si>
+    <t>2. What did Jenna and Max find inside the ancient shipwreck?</t>
+  </si>
+  <si>
+    <t>a) A treasure chest of gold
+b) Old maps and strange artifacts
+c) A secret message
+d) A new energy source</t>
+  </si>
+  <si>
+    <t>3. How did the discovery of the shipwrecks benefit Oceana?</t>
+  </si>
+  <si>
+    <t>a) In the Arctic Ocean
+b) On the moon
+c) In the Pacific Ocean
+d) On a mountaintop</t>
+  </si>
+  <si>
+    <t>a) It made Jenna famous
+b) It provided valuable resources
+c) It led to the construction of another city
+d) It stopped the sea levels from rising</t>
+  </si>
+  <si>
+    <t>1.What was Verdantia known for?</t>
+  </si>
+  <si>
+    <t>a) Its giant trees and fertile soil
+b) Its vast deserts
+c) Its advanced technology
+d) Its floating cities</t>
+  </si>
+  <si>
+    <t>2. What did Liam discover in the forest?</t>
+  </si>
+  <si>
+    <t>a) A hidden treasure
+b) A new species of animal
+c) A sick tree showing signs of decay
+d) A secret cave</t>
+  </si>
+  <si>
+    <t>3. How did the Galactic Gardeners save the trees from the fungus?</t>
+  </si>
+  <si>
+    <t>a) By cutting down the infected trees
+b) By relocating the trees
+c) By developing a special serum
+d) By using robots to clean the trees</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -502,10 +568,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -738,7 +804,110 @@
         <v>5</v>
       </c>
     </row>
+    <row r="14" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" t="s">
+        <v>50</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E18" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" t="s">
+        <v>52</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E19" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
option E was added
</commit_message>
<xml_diff>
--- a/psychopy_experiment/comp_materials/passage_qa/questionbank.xlsx
+++ b/psychopy_experiment/comp_materials/passage_qa/questionbank.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erang\Desktop\Reading_task\psychopy_experiment\comp_materials\passage_qa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E774C1A-7034-4B8B-8EE8-C48072A1B3F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3D1B720-55D2-4AB7-B520-D34C2B150DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -81,12 +81,6 @@
     <t>3. What script replaced Linear A after the destruction of the Minoan palaces?</t>
   </si>
   <si>
-    <t>A) Land-based political system
-B) Theocratic political system
-C) Democracy
-D) Sea-based political system</t>
-  </si>
-  <si>
     <t>d</t>
   </si>
   <si>
@@ -113,72 +107,6 @@
   </si>
   <si>
     <t>3. What term describes the rule of older men in Sparta?</t>
-  </si>
-  <si>
-    <t>A) Hieroglyphics
-B) Linear B
-C) Linear A
-D) Cuneiform</t>
-  </si>
-  <si>
-    <t>A) Hieroglyphics
-B) Linear B
-C) Cuneiform
-D) Greek alphabet</t>
-  </si>
-  <si>
-    <t>A) The rise of monarchies
-B) The abolition of free males
-C) The idea of free males being equal in status
-D) The establishment of feudalism</t>
-  </si>
-  <si>
-    <t>A) Democracy
-B) Oligarchy
-C) Tyranny
-D) Monarchy</t>
-  </si>
-  <si>
-    <t>A) Submission to a hierarchical order
-B) Pursuit of harmonious coexistence
-C) Emphasis on rebellious and independent spirit
-D) Reliance on established aristocratic traditions</t>
-  </si>
-  <si>
-    <t>A) Abundance of resources
-B) Scarce resources
-C) Political stability
-D) Military pressure</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A) Their agricultural practices 
-B) Their political systems 
-C) Their architectural styles
-D) Their distinctive way of life </t>
-  </si>
-  <si>
-    <t>A) Lack of historical records
-B) Reapplying old names to new settlements
-C) Limited archaeological evidence
-D) Inconsistent historical accounts</t>
-  </si>
-  <si>
-    <t>A) Perioeci
-B) Helots
-C) Spartiates
-D) Ephors</t>
-  </si>
-  <si>
-    <t>A) Achilles
-B) Heracles
-C) Odysseus
-D) Theseus</t>
-  </si>
-  <si>
-    <t>A) Democracy
-B) Monarchy
-C) Gerontocracy
-D) Oligarchy</t>
   </si>
   <si>
     <t>2. By the late sixth century BC, what did the vision of the ideal citizen of the city-state lead to?</t>
@@ -242,6 +170,90 @@
 b) By relocating the trees
 c) By developing a special serum
 d) By using robots to clean the trees</t>
+  </si>
+  <si>
+    <t>A) Democracy
+B) Monarchy
+C) Gerontocracy
+D) Oligarchy
+E) Aristocracy</t>
+  </si>
+  <si>
+    <t>A) Achilles
+B) Heracles
+C) Odysseus
+D) Theseus
+E) Apollo</t>
+  </si>
+  <si>
+    <t>A) Perioeci
+B) Helots
+C) Spartiates
+D) Ephors
+E) Metics</t>
+  </si>
+  <si>
+    <t>A) Lack of historical records
+B) Reapplying old names to new settlements
+C) Limited archaeological evidence
+D) Inconsistent historical accounts
+E) Fragmentary literary sources</t>
+  </si>
+  <si>
+    <t>A) Their agricultural practices 
+B) Their political systems 
+C) Their architectural styles
+D) Their distinct way of life 
+E) Their religious beliefs</t>
+  </si>
+  <si>
+    <t>A) Abundance of resources
+B) Scarce resources
+C) Political stability
+D) Military pressure
+E) Social inequality</t>
+  </si>
+  <si>
+    <t>A) Democracy
+B) Oligarchy
+C) Tyranny
+D) Monarchy
+E) Military rule</t>
+  </si>
+  <si>
+    <t>A) The rise of monarchies
+B) The abolition of free males
+C) The idea of free males being equal in status
+D) The establishment of feudalism
+E) The creation of democratic institutions</t>
+  </si>
+  <si>
+    <t>A) Hieroglyphics
+B) Linear B
+C) Cuneiform
+D) Greek alphabet
+E) Phoenician script</t>
+  </si>
+  <si>
+    <t>A) Hieroglyphics
+B) Linear B
+C) Linear A
+D) Cuneiform
+E) Phoenician alphabet</t>
+  </si>
+  <si>
+    <t>A) Land-based political system
+B) Theocratic political system
+C) Democracy
+D) Sea-based political system
+E) Aristocratic political system</t>
+  </si>
+  <si>
+    <t>A) Submission to a hierarchical order
+B) Pursuit of harmonious coexistence
+C) Emphasis on rebellious and independent spirit
+D) Reliance on established aristocratic traditions 
+E) Commitment to civic participation</t>
   </si>
 </sst>
 </file>
@@ -570,8 +582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -600,7 +612,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -611,13 +623,13 @@
         <v>15</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" t="s">
         <v>18</v>
       </c>
-      <c r="E2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -628,13 +640,13 @@
         <v>16</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="E3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -645,13 +657,13 @@
         <v>17</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="E4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -659,16 +671,16 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="E5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -676,16 +688,16 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="E6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -693,16 +705,16 @@
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
       <c r="E7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -710,16 +722,16 @@
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="E8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -727,16 +739,16 @@
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="E9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -744,16 +756,16 @@
         <v>3</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="E10" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -761,16 +773,16 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="E11" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -778,16 +790,16 @@
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="E12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -795,10 +807,10 @@
         <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E13" t="s">
         <v>5</v>
@@ -806,16 +818,16 @@
     </row>
     <row r="14" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="B14" t="s">
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="E14" t="s">
         <v>5</v>
@@ -823,16 +835,16 @@
     </row>
     <row r="15" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="B15" t="s">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="E15" t="s">
         <v>11</v>
@@ -840,16 +852,16 @@
     </row>
     <row r="16" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="B16" t="s">
         <v>3</v>
       </c>
       <c r="C16" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="E16" t="s">
         <v>11</v>
@@ -857,16 +869,16 @@
     </row>
     <row r="17" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="B17" t="s">
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="E17" t="s">
         <v>4</v>
@@ -874,16 +886,16 @@
     </row>
     <row r="18" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="B18" t="s">
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="E18" t="s">
         <v>5</v>
@@ -891,16 +903,16 @@
     </row>
     <row r="19" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="B19" t="s">
         <v>3</v>
       </c>
       <c r="C19" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="E19" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
4 more passages were added
</commit_message>
<xml_diff>
--- a/psychopy_experiment/comp_materials/passage_qa/questionbank.xlsx
+++ b/psychopy_experiment/comp_materials/passage_qa/questionbank.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erang\Desktop\Reading_task\psychopy_experiment\comp_materials\passage_qa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3D1B720-55D2-4AB7-B520-D34C2B150DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3E3B5FF-38FC-435B-A8D8-A8E6335363B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="83">
   <si>
     <t>R1</t>
   </si>
@@ -254,6 +254,141 @@
 C) Emphasis on rebellious and independent spirit
 D) Reliance on established aristocratic traditions 
 E) Commitment to civic participation</t>
+  </si>
+  <si>
+    <t>R5</t>
+  </si>
+  <si>
+    <t>1. The bathtub in the palace at Pylos was made of what material?</t>
+  </si>
+  <si>
+    <t>2. The hero shrine at Therapne was made for whom?</t>
+  </si>
+  <si>
+    <t>3. Who was falsely accused by Queen Antaea of attacking her?</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>A) Telemachus
+B) Proitos
+C) Menelaus
+D) Nestor
+E) Bellerophon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A) Achilles
+B) Odysseus
+C) Agamemnon
+D) Hector
+E) Helen </t>
+  </si>
+  <si>
+    <t>A) Marble
+B) Bronze
+C) Stone
+D) Terra-cotta
+E) Wood</t>
+  </si>
+  <si>
+    <t>R6</t>
+  </si>
+  <si>
+    <t>A) Olympion
+B) Delphinion
+C) Apollonion
+D) Hellenion
+E) Pythion</t>
+  </si>
+  <si>
+    <t>A) Nemean Games
+B) Isthmian Games
+C) Pythian Games
+D) Panathenaic Games
+E) Corinthian Games</t>
+  </si>
+  <si>
+    <t>A) Wrestling
+B) Musical
+C) Running
+D) Javelin throwing
+E) Chariot racing</t>
+  </si>
+  <si>
+    <t>1. What was the primary focus of the first competitions at Delphi?</t>
+  </si>
+  <si>
+    <t>2. Name one more game mentioned in the passage besides the Olympic Games.</t>
+  </si>
+  <si>
+    <t>3. What was the name of the shared shrine built by Greeks in Naucratis?</t>
+  </si>
+  <si>
+    <t>R7</t>
+  </si>
+  <si>
+    <t>1. What started the French wine industry?</t>
+  </si>
+  <si>
+    <t>2. Who fell in love with Cyrene according to Pindar’s poem?</t>
+  </si>
+  <si>
+    <t>3. King Arcesilas of Cyrene won which race?</t>
+  </si>
+  <si>
+    <t>A) Greeks bringing grapevines to Massalia
+B) Romans introducing winemaking techniques
+C) Local Ligurian practices
+D) Phoenician traders bringing grapes
+E) Egyptian agricultural influence</t>
+  </si>
+  <si>
+    <t>A) Zeus
+B) Heracles
+C) Apollo
+D) Poseidon
+E) Ares</t>
+  </si>
+  <si>
+    <t>A) Hoplite race
+B) Chariot race
+C) Long jump
+D) Javelin throw
+E) Wrestling</t>
+  </si>
+  <si>
+    <t>R8</t>
+  </si>
+  <si>
+    <t>Who is considered by some to be the first known case of PTSD in western literary tradition?</t>
+  </si>
+  <si>
+    <t>What qualities contributed to Sparta’s success in hoplite warfare?</t>
+  </si>
+  <si>
+    <t>How did Spartans react to the death of their kings?</t>
+  </si>
+  <si>
+    <t>A) Leonidas
+B) Brasidas
+C) Clearchus
+D) Gylippus
+E) Heracles</t>
+  </si>
+  <si>
+    <t>A) Superior weaponry
+B) Large armies
+C) Advanced technology
+D) Morale and organization
+E) Naval dominance</t>
+  </si>
+  <si>
+    <t>A) Paused activities
+B) Held feasts
+C) Declared holidays
+D) Increased training
+E) Expanded territory</t>
   </si>
 </sst>
 </file>
@@ -580,10 +715,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -918,6 +1053,210 @@
         <v>5</v>
       </c>
     </row>
+    <row r="20" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" t="s">
+        <v>55</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>54</v>
+      </c>
+      <c r="B21" t="s">
+        <v>2</v>
+      </c>
+      <c r="C21" t="s">
+        <v>56</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E21" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>54</v>
+      </c>
+      <c r="B22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" t="s">
+        <v>57</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E22" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>62</v>
+      </c>
+      <c r="B23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23" t="s">
+        <v>66</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E23" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>62</v>
+      </c>
+      <c r="B24" t="s">
+        <v>2</v>
+      </c>
+      <c r="C24" t="s">
+        <v>67</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E24" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>62</v>
+      </c>
+      <c r="B25" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25" t="s">
+        <v>68</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E25" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>69</v>
+      </c>
+      <c r="B26" t="s">
+        <v>1</v>
+      </c>
+      <c r="C26" t="s">
+        <v>70</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E26" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>69</v>
+      </c>
+      <c r="B27" t="s">
+        <v>2</v>
+      </c>
+      <c r="C27" t="s">
+        <v>71</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E27" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>69</v>
+      </c>
+      <c r="B28" t="s">
+        <v>3</v>
+      </c>
+      <c r="C28" t="s">
+        <v>72</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E28" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>76</v>
+      </c>
+      <c r="B29" t="s">
+        <v>1</v>
+      </c>
+      <c r="C29" t="s">
+        <v>77</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E29" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>76</v>
+      </c>
+      <c r="B30" t="s">
+        <v>2</v>
+      </c>
+      <c r="C30" t="s">
+        <v>78</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E30" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>76</v>
+      </c>
+      <c r="B31" t="s">
+        <v>3</v>
+      </c>
+      <c r="C31" t="s">
+        <v>79</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E31" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
bat file was added
</commit_message>
<xml_diff>
--- a/psychopy_experiment/comp_materials/passage_qa/questionbank.xlsx
+++ b/psychopy_experiment/comp_materials/passage_qa/questionbank.xlsx
@@ -8,24 +8,35 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erang\Desktop\Reading_task\psychopy_experiment\comp_materials\passage_qa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4749426F-D89B-445A-A7B5-68E1E7315CAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2096C38C-2DE4-41F5-8624-9DE33BDDA45F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="83">
   <si>
     <t>R1</t>
   </si>
@@ -259,54 +270,10 @@
     <t>R5</t>
   </si>
   <si>
-    <t>1. The bathtub in the palace at Pylos was made of what material?</t>
-  </si>
-  <si>
     <t>2. The hero shrine at Therapne was made for whom?</t>
   </si>
   <si>
-    <t>3. Who was falsely accused by Queen Antaea of attacking her?</t>
-  </si>
-  <si>
-    <t>e</t>
-  </si>
-  <si>
-    <t>A) Telemachus
-B) Proitos
-C) Menelaus
-D) Nestor
-E) Bellerophon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A) Achilles
-B) Odysseus
-C) Agamemnon
-D) Hector
-E) Helen </t>
-  </si>
-  <si>
-    <t>A) Marble
-B) Bronze
-C) Stone
-D) Terra-cotta
-E) Wood</t>
-  </si>
-  <si>
     <t>R6</t>
-  </si>
-  <si>
-    <t>A) Olympion
-B) Delphinion
-C) Apollonion
-D) Hellenion
-E) Pythion</t>
-  </si>
-  <si>
-    <t>A) Nemean Games
-B) Isthmian Games
-C) Pythian Games
-D) Panathenaic Games
-E) Corinthian Games</t>
   </si>
   <si>
     <t>A) Wrestling
@@ -319,29 +286,7 @@
     <t>1. What was the primary focus of the first competitions at Delphi?</t>
   </si>
   <si>
-    <t>2. Name one more game mentioned in the passage besides the Olympic Games.</t>
-  </si>
-  <si>
-    <t>3. What was the name of the shared shrine built by Greeks in Naucratis?</t>
-  </si>
-  <si>
     <t>R7</t>
-  </si>
-  <si>
-    <t>1. What started the French wine industry?</t>
-  </si>
-  <si>
-    <t>2. Who fell in love with Cyrene according to Pindar’s poem?</t>
-  </si>
-  <si>
-    <t>3. King Arcesilas of Cyrene won which race?</t>
-  </si>
-  <si>
-    <t>A) Greeks bringing grapevines to Massalia
-B) Romans introducing winemaking techniques
-C) Local Ligurian practices
-D) Phoenician traders bringing grapes
-E) Egyptian agricultural influence</t>
   </si>
   <si>
     <t>A) Zeus
@@ -351,21 +296,7 @@
 E) Ares</t>
   </si>
   <si>
-    <t>A) Hoplite race
-B) Chariot race
-C) Long jump
-D) Javelin throw
-E) Wrestling</t>
-  </si>
-  <si>
     <t>R8</t>
-  </si>
-  <si>
-    <t>A) Leonidas
-B) Brasidas
-C) Clearchus
-D) Gylippus
-E) Heracles</t>
   </si>
   <si>
     <t>A) Superior weaponry
@@ -375,20 +306,100 @@
 E) Naval dominance</t>
   </si>
   <si>
-    <t>A) Paused activities
-B) Held feasts
-C) Declared holidays
-D) Increased training
-E) Expanded territory</t>
-  </si>
-  <si>
-    <t>1.Who is considered by some to be the first known case of PTSD in western literary tradition?</t>
-  </si>
-  <si>
-    <t>2.What qualities contributed to Sparta’s success in hoplite warfare?</t>
-  </si>
-  <si>
-    <t>3.How did Spartans react to the death of their kings?</t>
+    <t>A) They had luxurious items indicating wealth and comfort
+B) They were built primarily for defense
+C) They were simple and lacked decoration
+D) They focused on agricultural storage
+E) They were designed for religious ceremonies only</t>
+  </si>
+  <si>
+    <t>A) Achilles
+B) Odysseus
+C) Agamemnon
+D) Hector
+E) Helen</t>
+  </si>
+  <si>
+    <t>A) Leadership
+B) Wealth
+C) False accusation
+D) Military skills
+E) Diplomacy</t>
+  </si>
+  <si>
+    <t>A) Promoted economic growth
+B) Established military alliances
+C) Managed relationships
+D) Enforced legal systems
+E) Expanded territories</t>
+  </si>
+  <si>
+    <t>A) Trade in markets
+B) Fight in wars
+C) Participate in games
+D) Hold religious festivals
+E) Attend political assemblies</t>
+  </si>
+  <si>
+    <t>A) Wealth and luxury
+B) Agricultural skills
+C) Strength and heroism
+D) Peace and coexistence
+E) Democratic principles</t>
+  </si>
+  <si>
+    <t>A) During peace times
+B) When spending his fortune
+C) When fighting
+D) When forming close relationships
+E) When following orders</t>
+  </si>
+  <si>
+    <t>A) Lack of weapons
+B) Poor weather
+C) Insufficient troops
+D) Religious omens
+E) Political decisions</t>
+  </si>
+  <si>
+    <t>1. How did the features of Mycenaean palaces reflect the priorities of the royal family?</t>
+  </si>
+  <si>
+    <t>3. What is interesting about the Queen of Tiryns?</t>
+  </si>
+  <si>
+    <t>2. How did Panhellenic shrines serve Greece?</t>
+  </si>
+  <si>
+    <t>3. What did the Greeks do to gather yearly?</t>
+  </si>
+  <si>
+    <t>1. What does the marriage in the passage with the French wine industry symbolize?</t>
+  </si>
+  <si>
+    <t>1. When was Clearchus happy?</t>
+  </si>
+  <si>
+    <t>3. What would stop Spartans from going to battle?</t>
+  </si>
+  <si>
+    <t>2. What qualities contributed to Spartan's success in hoplite warfare?</t>
+  </si>
+  <si>
+    <t>3. Who fell in love with Cyrene according to Pindar's poem?</t>
+  </si>
+  <si>
+    <t>2. What values are reflected in Pindara's portrayal of Cyrene?</t>
+  </si>
+  <si>
+    <t>A) Greek conquest
+B) Decline of Ligurians
+C) New Greek dynasty
+D) Union of cultures
+E) Political control</t>
+  </si>
+  <si>
+    <t>e</t>
   </si>
 </sst>
 </file>
@@ -717,8 +728,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -760,8 +771,9 @@
       <c r="D2" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E2" t="s">
-        <v>18</v>
+      <c r="E2" t="str">
+        <f>LOWER("d")</f>
+        <v>d</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="72" x14ac:dyDescent="0.3">
@@ -777,8 +789,9 @@
       <c r="D3" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E3" t="s">
-        <v>5</v>
+      <c r="E3" t="str">
+        <f>LOWER("c")</f>
+        <v>c</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="72" x14ac:dyDescent="0.3">
@@ -1053,7 +1066,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>54</v>
       </c>
@@ -1061,13 +1074,13 @@
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E20" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="72" x14ac:dyDescent="0.3">
@@ -1078,13 +1091,13 @@
         <v>2</v>
       </c>
       <c r="C21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="E21" t="s">
-        <v>58</v>
+        <v>82</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="72" x14ac:dyDescent="0.3">
@@ -1095,27 +1108,27 @@
         <v>3</v>
       </c>
       <c r="C22" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="E22" t="s">
-        <v>58</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B23" t="s">
         <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="E23" t="s">
         <v>11</v>
@@ -1123,16 +1136,16 @@
     </row>
     <row r="24" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B24" t="s">
         <v>2</v>
       </c>
       <c r="C24" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E24" t="s">
         <v>5</v>
@@ -1140,50 +1153,50 @@
     </row>
     <row r="25" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B25" t="s">
         <v>3</v>
       </c>
       <c r="C25" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="E25" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="B26" t="s">
         <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="E26" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="B27" t="s">
         <v>2</v>
       </c>
       <c r="C27" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="E27" t="s">
         <v>5</v>
@@ -1191,33 +1204,33 @@
     </row>
     <row r="28" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="B28" t="s">
         <v>3</v>
       </c>
       <c r="C28" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="E28" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="B29" t="s">
         <v>1</v>
       </c>
       <c r="C29" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="E29" t="s">
         <v>5</v>
@@ -1225,16 +1238,16 @@
     </row>
     <row r="30" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="B30" t="s">
         <v>2</v>
       </c>
       <c r="C30" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="E30" t="s">
         <v>18</v>
@@ -1242,19 +1255,19 @@
     </row>
     <row r="31" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="B31" t="s">
         <v>3</v>
       </c>
       <c r="C31" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="E31" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>